<commit_message>
added auth to users index
</commit_message>
<xml_diff>
--- a/doc/sprint3_burndown.xlsx
+++ b/doc/sprint3_burndown.xlsx
@@ -530,10 +530,10 @@
                   <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>9.0</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>9.0</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>4.0</c:v>
@@ -557,11 +557,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1961620976"/>
-        <c:axId val="1961625632"/>
+        <c:axId val="1434376896"/>
+        <c:axId val="1468498416"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1961620976"/>
+        <c:axId val="1434376896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="42655.0"/>
@@ -676,14 +676,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1961625632"/>
+        <c:crossAx val="1468498416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1.0"/>
         <c:minorUnit val="1.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1961625632"/>
+        <c:axId val="1468498416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -801,7 +801,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1961620976"/>
+        <c:crossAx val="1434376896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1738,8 +1738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1950,7 +1950,7 @@
         <v>9</v>
       </c>
       <c r="C19">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -1961,7 +1961,7 @@
         <v>4</v>
       </c>
       <c r="C20">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>